<commit_message>
Game Web APIs finished
</commit_message>
<xml_diff>
--- a/scripts/game_examples.xlsx
+++ b/scripts/game_examples.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Combination" sheetId="5" r:id="rId1"/>
@@ -17,8 +17,22 @@
     <sheet name="Equivalence" sheetId="1" r:id="rId3"/>
     <sheet name="Estimation" sheetId="7" r:id="rId4"/>
     <sheet name="TrueFalse" sheetId="8" r:id="rId5"/>
+    <sheet name="FillBlank" sheetId="10" r:id="rId6"/>
+    <sheet name="Short Choice" sheetId="12" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="Z_A88A978D_EDD0_DB4B_AF38_97F4E8575985_.wvu.Cols" localSheetId="0" hidden="1">Combination!$C:$C,Combination!$E:$F,Combination!$H:$I,Combination!$K:$K,Combination!$M:$M</definedName>
+    <definedName name="Z_A88A978D_EDD0_DB4B_AF38_97F4E8575985_.wvu.Cols" localSheetId="1" hidden="1">Comparision!$C:$C,Comparision!$E:$F,Comparision!$H:$I,Comparision!$K:$K,Comparision!$M:$M</definedName>
+    <definedName name="Z_A88A978D_EDD0_DB4B_AF38_97F4E8575985_.wvu.Cols" localSheetId="2" hidden="1">Equivalence!$C:$C,Equivalence!$E:$F,Equivalence!$H:$I,Equivalence!$K:$K,Equivalence!$M:$M</definedName>
+    <definedName name="Z_A88A978D_EDD0_DB4B_AF38_97F4E8575985_.wvu.Cols" localSheetId="3" hidden="1">Estimation!$C:$C,Estimation!$E:$F,Estimation!$H:$I,Estimation!$K:$K,Estimation!$M:$M</definedName>
+    <definedName name="Z_A88A978D_EDD0_DB4B_AF38_97F4E8575985_.wvu.Cols" localSheetId="5" hidden="1">FillBlank!$C:$C,FillBlank!$E:$F,FillBlank!$H:$I,FillBlank!$K:$K,FillBlank!$M:$M</definedName>
+    <definedName name="Z_A88A978D_EDD0_DB4B_AF38_97F4E8575985_.wvu.Cols" localSheetId="6" hidden="1">'Short Choice'!$C:$C,'Short Choice'!$E:$F,'Short Choice'!$H:$I,'Short Choice'!$K:$K,'Short Choice'!$M:$M</definedName>
+    <definedName name="Z_A88A978D_EDD0_DB4B_AF38_97F4E8575985_.wvu.Cols" localSheetId="4" hidden="1">TrueFalse!$C:$C,TrueFalse!$E:$F,TrueFalse!$H:$I,TrueFalse!$K:$K,TrueFalse!$M:$M</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
+  <customWorkbookViews>
+    <customWorkbookView name="150% zoomed out" guid="{A88A978D-EDD0-DB4B-AF38-97F4E8575985}" windowWidth="1440" windowHeight="714" tabRatio="500" activeSheetId="9"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="164">
   <si>
     <t>C07</t>
   </si>
@@ -159,21 +173,6 @@
     <t>Estimation</t>
   </si>
   <si>
-    <t>\\root{4}</t>
-  </si>
-  <si>
-    <t>\\root{10}</t>
-  </si>
-  <si>
-    <t>\\root{16}</t>
-  </si>
-  <si>
-    <t>\\root{37}</t>
-  </si>
-  <si>
-    <t>\\root{99}</t>
-  </si>
-  <si>
     <t>C06</t>
   </si>
   <si>
@@ -234,109 +233,310 @@
     <t>TrueFalse</t>
   </si>
   <si>
-    <t>(–5) \\times (–7) is a negative integer</t>
-  </si>
-  <si>
-    <t>(2) \\times (–4) is a negative integer</t>
-  </si>
-  <si>
-    <t>(-2) \\times (–4) is a positive integer</t>
-  </si>
-  <si>
-    <t>(-1) \\times (4) is a positive integer</t>
-  </si>
-  <si>
-    <t>(–5) \\times (–7) is same as (–7) \\times (–5)</t>
-  </si>
-  <si>
-    <t>(–4) \\times (–1) is same as (1) \\times (4)</t>
-  </si>
-  <si>
-    <t>\\frac{10}{100}</t>
-  </si>
-  <si>
-    <t>\\frac{20}{100}</t>
-  </si>
-  <si>
-    <t>\\frac{1}{10}</t>
-  </si>
-  <si>
-    <t>\\frac{3}{10}</t>
-  </si>
-  <si>
-    <t>\\frac{2}{20}</t>
-  </si>
-  <si>
-    <t>\\frac{4}{40}</t>
-  </si>
-  <si>
-    <t>\\frac{1}{1000}</t>
-  </si>
-  <si>
-    <t>\\frac{10}{1000}</t>
-  </si>
-  <si>
-    <t>\\frac{100}{10}</t>
-  </si>
-  <si>
-    <t>\\frac{9}{90}</t>
-  </si>
-  <si>
-    <t>\\frac{25}{100}</t>
-  </si>
-  <si>
-    <t>\\frac{1}{4}</t>
-  </si>
-  <si>
-    <t>\\frac{3}{12}</t>
-  </si>
-  <si>
-    <t>\\frac{10}{40}</t>
-  </si>
-  <si>
-    <t>\\frac{4}{41}</t>
-  </si>
-  <si>
-    <t>\\frac{40}{1000}</t>
-  </si>
-  <si>
-    <t>\\frac{4}{16}</t>
-  </si>
-  <si>
-    <t>\\frac{40}{160}</t>
-  </si>
-  <si>
-    <t>\\frac{6}{24}</t>
-  </si>
-  <si>
-    <t>\\frac{40}{100}</t>
-  </si>
-  <si>
-    <t>\\frac{2}{5}</t>
-  </si>
-  <si>
-    <t>\\frac{4}{10}</t>
-  </si>
-  <si>
-    <t>\\frac{16}{40}</t>
-  </si>
-  <si>
-    <t>\\frac{4}{11}</t>
-  </si>
-  <si>
-    <t>\\frac{400}{1000}</t>
-  </si>
-  <si>
-    <t>\\frac{8}{20}</t>
-  </si>
-  <si>
-    <t>\\frac{40}{110}</t>
-  </si>
-  <si>
-    <t>\\frac{6}{15}</t>
-  </si>
-  <si>
     <t>Square Roots</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Algebra</t>
+  </si>
+  <si>
+    <t>algebra</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Algebraic Expressions and Identities</t>
+  </si>
+  <si>
+    <t>algebraic-expressions-and-identities</t>
+  </si>
+  <si>
+    <t>AEI</t>
+  </si>
+  <si>
+    <t>Standard Identities</t>
+  </si>
+  <si>
+    <t>standard-identities</t>
+  </si>
+  <si>
+    <t>FillBlank</t>
+  </si>
+  <si>
+    <t>(a+b)</t>
+  </si>
+  <si>
+    <t>(a-b)</t>
+  </si>
+  <si>
+    <t>2ab</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>Question\_name</t>
+  </si>
+  <si>
+    <t>Hint\_text</t>
+  </si>
+  <si>
+    <t>(a – b) \_\_\_\_\_\_\_\_\_ = a^{2} – 2ab + b^{2}</t>
+  </si>
+  <si>
+    <t>a^{2} – b^{2} = (a + b ) \_\_\_\_\_\_\_\_\_\_.</t>
+  </si>
+  <si>
+    <t>(a – b)^{2} + \_\_\_\_\_\_\_\_\_\_\_\_ = a^{2} – b^{2}</t>
+  </si>
+  <si>
+    <t>(a + b)^{2} – \_\_\_\_\_\_\_\_\_\_\_ =a^{2}  +b^{2}</t>
+  </si>
+  <si>
+    <t>(x + a) (x + b) = x^{2} + (a + b) x + \_\_\_\_\_\_\_\_.</t>
+  </si>
+  <si>
+    <t>Change in Percent</t>
+  </si>
+  <si>
+    <t>change-in-percent</t>
+  </si>
+  <si>
+    <t>Find increase/decrease per cent</t>
+  </si>
+  <si>
+    <t>On Sunday $$845$$ people went to zoo. On Monday only $$169$$ people went to zoo. What is the percentage decrease in people visiting zoo on Monday ?</t>
+  </si>
+  <si>
+    <t>$$50\%$$</t>
+  </si>
+  <si>
+    <t>$$60\%$$</t>
+  </si>
+  <si>
+    <t>$$70\%$$</t>
+  </si>
+  <si>
+    <t>$$80\%$$</t>
+  </si>
+  <si>
+    <t>Find the new value if $$300$$ decreased by $$30\%$$</t>
+  </si>
+  <si>
+    <t>$$220$$</t>
+  </si>
+  <si>
+    <t>$$100$$</t>
+  </si>
+  <si>
+    <t>$$150$$</t>
+  </si>
+  <si>
+    <t>$$210$$</t>
+  </si>
+  <si>
+    <t>A number is increased from $$125$$ to $$150$$, find the percentage increase.</t>
+  </si>
+  <si>
+    <t>$$10$$%</t>
+  </si>
+  <si>
+    <t>$$20$$%</t>
+  </si>
+  <si>
+    <t>$$30$$%</t>
+  </si>
+  <si>
+    <t>None of these&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>A number is decreased from 125 to 100, find the percentage decrease.</t>
+  </si>
+  <si>
+    <t>The percent increase from $$6$$ to $$15$$ is equal to the percent increase from $$15$$ to&amp;#160;&lt;span&gt;&lt;br/&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;$$30$$&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;$$19.5$$&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>$$37.5$$</t>
+  </si>
+  <si>
+    <t>&lt;span&gt;$$27.5$$&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>A triangle is to be changed by increasing the length of its base by $$40$$% and decreasing&amp;#160;the length of its height by $$40$$%. What is the increase or decrease in the area of the triangle?</t>
+  </si>
+  <si>
+    <t>It will increase by $$40$$%</t>
+  </si>
+  <si>
+    <t>It will increase by $$16$$%</t>
+  </si>
+  <si>
+    <t>It will not change</t>
+  </si>
+  <si>
+    <t>It will decrease by $$16$$%</t>
+  </si>
+  <si>
+    <t>The price of rice is increased from Rs. $$10$$ to Rs. $$12.50$$ per kg. Find the percentage increase in price.</t>
+  </si>
+  <si>
+    <t>$$10\%$$</t>
+  </si>
+  <si>
+    <t>$$20\%$$</t>
+  </si>
+  <si>
+    <t>$$25\%$$</t>
+  </si>
+  <si>
+    <t>$$15\%$$</t>
+  </si>
+  <si>
+    <t>A number increased from $$120$$ to $$150$$. By what percent, of its original value, did this number increase?</t>
+  </si>
+  <si>
+    <t>$$30\%$$</t>
+  </si>
+  <si>
+    <t>10%</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>(–5) \times (–7) is a negative integer</t>
+  </si>
+  <si>
+    <t>(2) \times (–4) is a negative integer</t>
+  </si>
+  <si>
+    <t>(-2) \times (–4) is a positive integer</t>
+  </si>
+  <si>
+    <t>(-1) \times (4) is a positive integer</t>
+  </si>
+  <si>
+    <t>(–5) \times (–7) is same as (–7) \times (–5)</t>
+  </si>
+  <si>
+    <t>(–4) \times (–1) is same as (1) \times (4)</t>
+  </si>
+  <si>
+    <t>\root{4}</t>
+  </si>
+  <si>
+    <t>\root{10}</t>
+  </si>
+  <si>
+    <t>\root{16}</t>
+  </si>
+  <si>
+    <t>\root{37}</t>
+  </si>
+  <si>
+    <t>\root{99}</t>
+  </si>
+  <si>
+    <t>\frac{10}{100}</t>
+  </si>
+  <si>
+    <t>\frac{20}{100}</t>
+  </si>
+  <si>
+    <t>\frac{1}{10}</t>
+  </si>
+  <si>
+    <t>\frac{3}{10}</t>
+  </si>
+  <si>
+    <t>\frac{2}{20}</t>
+  </si>
+  <si>
+    <t>\frac{4}{40}</t>
+  </si>
+  <si>
+    <t>\frac{1}{1000}</t>
+  </si>
+  <si>
+    <t>\frac{10}{1000}</t>
+  </si>
+  <si>
+    <t>\frac{100}{10}</t>
+  </si>
+  <si>
+    <t>\frac{9}{90}</t>
+  </si>
+  <si>
+    <t>\frac{25}{100}</t>
+  </si>
+  <si>
+    <t>\frac{1}{4}</t>
+  </si>
+  <si>
+    <t>\frac{3}{12}</t>
+  </si>
+  <si>
+    <t>\frac{10}{40}</t>
+  </si>
+  <si>
+    <t>\frac{4}{41}</t>
+  </si>
+  <si>
+    <t>\frac{40}{1000}</t>
+  </si>
+  <si>
+    <t>\frac{4}{16}</t>
+  </si>
+  <si>
+    <t>\frac{40}{160}</t>
+  </si>
+  <si>
+    <t>\frac{6}{24}</t>
+  </si>
+  <si>
+    <t>\frac{40}{100}</t>
+  </si>
+  <si>
+    <t>\frac{2}{5}</t>
+  </si>
+  <si>
+    <t>\frac{4}{10}</t>
+  </si>
+  <si>
+    <t>\frac{16}{40}</t>
+  </si>
+  <si>
+    <t>\frac{4}{11}</t>
+  </si>
+  <si>
+    <t>\frac{400}{1000}</t>
+  </si>
+  <si>
+    <t>\frac{8}{20}</t>
+  </si>
+  <si>
+    <t>\frac{40}{110}</t>
+  </si>
+  <si>
+    <t>\frac{6}{15}</t>
+  </si>
+  <si>
+    <t>ShortChoice</t>
   </si>
 </sst>
 </file>
@@ -378,10 +578,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -659,25 +861,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ6"/>
+  <dimension ref="A1:AM6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -730,9 +932,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -750,25 +952,25 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>34</v>
@@ -787,23 +989,34 @@
         <v>1</v>
       </c>
       <c r="T2" s="2">
+        <v>1</v>
+      </c>
+      <c r="U2" s="2">
+        <v>2</v>
+      </c>
+      <c r="V2" s="2">
         <v>0.1</v>
       </c>
-      <c r="U2" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="V2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AJ2" s="2"/>
-    </row>
-    <row r="3" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="W2" s="2">
+        <v>4</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AM2" s="2"/>
+    </row>
+    <row r="3" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -821,25 +1034,25 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>34</v>
@@ -855,26 +1068,37 @@
         <v>10</v>
       </c>
       <c r="S3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3" s="2">
+        <v>1</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2">
         <v>0.1</v>
       </c>
-      <c r="U3" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="V3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AJ3" s="2"/>
-    </row>
-    <row r="4" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="W3" s="2">
+        <v>3</v>
+      </c>
+      <c r="X3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AM3" s="2"/>
+    </row>
+    <row r="4" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -892,25 +1116,25 @@
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>34</v>
@@ -926,26 +1150,37 @@
         <v>10</v>
       </c>
       <c r="S4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T4" s="2">
+        <v>1</v>
+      </c>
+      <c r="U4" s="2">
+        <v>1</v>
+      </c>
+      <c r="V4" s="2">
         <v>0.1</v>
       </c>
-      <c r="U4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="V4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AJ4" s="2"/>
-    </row>
-    <row r="5" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="W4" s="2">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AM4" s="2"/>
+    </row>
+    <row r="5" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -963,25 +1198,25 @@
         <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>34</v>
@@ -996,18 +1231,30 @@
         <v>10</v>
       </c>
       <c r="S5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5" s="2">
+        <v>1</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
         <v>0.1</v>
       </c>
-      <c r="U5" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="W5" s="2">
+        <v>4</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
@@ -1025,25 +1272,25 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>34</v>
@@ -1058,16 +1305,34 @@
         <v>10</v>
       </c>
       <c r="S6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6" s="2">
+        <v>1</v>
+      </c>
+      <c r="U6" s="2">
+        <v>2</v>
+      </c>
+      <c r="V6" s="2">
         <v>0.1</v>
       </c>
-      <c r="U6" s="2">
-        <v>0.2</v>
+      <c r="W6" s="2">
+        <v>3</v>
+      </c>
+      <c r="X6" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{A88A978D-EDD0-DB4B-AF38-97F4E8575985}" scale="150" hiddenColumns="1" topLeftCell="L1">
+      <selection activeCell="R4" sqref="R4"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1076,18 +1341,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ4"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.83203125" customWidth="1"/>
   </cols>
@@ -1147,7 +1412,7 @@
     </row>
     <row r="2" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1165,25 +1430,25 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>33</v>
@@ -1231,7 +1496,7 @@
     </row>
     <row r="3" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -1249,25 +1514,25 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>33</v>
@@ -1315,7 +1580,7 @@
     </row>
     <row r="4" spans="1:36" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -1333,25 +1598,25 @@
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>33</v>
@@ -1398,6 +1663,12 @@
       <c r="AJ4" s="2"/>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{A88A978D-EDD0-DB4B-AF38-97F4E8575985}" scale="150" hiddenColumns="1" topLeftCell="Q1">
+      <selection activeCell="A3" sqref="A3:N4"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1406,21 +1677,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.83203125" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="17" x14ac:dyDescent="0.2">
@@ -1469,7 +1741,7 @@
       <c r="O1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>28</v>
       </c>
       <c r="Q1" s="2" t="s">
@@ -1522,68 +1794,68 @@
       <c r="O2" s="2">
         <v>1</v>
       </c>
-      <c r="P2" s="1">
-        <v>0.1</v>
+      <c r="P2" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="U2">
         <v>0</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
       <c r="W2">
         <v>1</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="Y2">
         <v>0</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
       <c r="AA2">
         <v>1</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="AC2">
         <v>1</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AG2">
         <v>1</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="AI2">
         <v>0</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>82</v>
+        <v>144</v>
       </c>
       <c r="AK2">
         <v>0</v>
@@ -1635,68 +1907,68 @@
       <c r="O3">
         <v>2</v>
       </c>
-      <c r="P3" s="1">
-        <v>0.25</v>
+      <c r="P3" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>83</v>
+        <v>145</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="U3">
         <v>0</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>84</v>
+        <v>146</v>
       </c>
       <c r="W3">
         <v>1</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>85</v>
+        <v>147</v>
       </c>
       <c r="Y3">
         <v>1</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="AA3">
         <v>1</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>87</v>
+        <v>149</v>
       </c>
       <c r="AC3">
         <v>0</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>88</v>
+        <v>150</v>
       </c>
       <c r="AE3">
         <v>1</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>89</v>
+        <v>151</v>
       </c>
       <c r="AG3">
         <v>1</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>90</v>
+        <v>152</v>
       </c>
       <c r="AI3">
         <v>1</v>
       </c>
       <c r="AJ3" s="2" t="s">
-        <v>91</v>
+        <v>153</v>
       </c>
       <c r="AK3">
         <v>1</v>
@@ -1748,74 +2020,80 @@
       <c r="O4">
         <v>3</v>
       </c>
-      <c r="P4" s="1">
-        <v>0.4</v>
+      <c r="P4" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="S4">
         <v>1</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="U4">
         <v>0</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>93</v>
+        <v>155</v>
       </c>
       <c r="W4">
         <v>1</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>94</v>
+        <v>156</v>
       </c>
       <c r="Y4">
         <v>1</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
       <c r="AA4">
         <v>1</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="AC4">
         <v>0</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="AE4">
         <v>1</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="AG4">
         <v>1</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
       <c r="AI4">
         <v>0</v>
       </c>
       <c r="AJ4" s="2" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="AK4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{A88A978D-EDD0-DB4B-AF38-97F4E8575985}" scale="150" hiddenColumns="1" topLeftCell="J1">
+      <selection activeCell="R2" sqref="R2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1825,17 +2103,17 @@
   <dimension ref="A1:AJ6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="R6" sqref="A1:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.83203125" customWidth="1"/>
   </cols>
@@ -1922,7 +2200,7 @@
         <v>38</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>40</v>
@@ -1940,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2">
@@ -1987,7 +2265,7 @@
         <v>38</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>40</v>
@@ -2005,7 +2283,7 @@
         <v>2</v>
       </c>
       <c r="P3" t="s">
-        <v>43</v>
+        <v>131</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2">
@@ -2052,7 +2330,7 @@
         <v>38</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>40</v>
@@ -2070,7 +2348,7 @@
         <v>3</v>
       </c>
       <c r="P4" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2">
@@ -2117,7 +2395,7 @@
         <v>38</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>40</v>
@@ -2135,7 +2413,7 @@
         <v>4</v>
       </c>
       <c r="P5" t="s">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="R5" s="2">
         <v>6.08</v>
@@ -2173,7 +2451,7 @@
         <v>38</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>40</v>
@@ -2191,7 +2469,7 @@
         <v>5</v>
       </c>
       <c r="P6" t="s">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="R6" s="2">
         <v>9.94</v>
@@ -2201,8 +2479,14 @@
       <c r="U6" s="2"/>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{A88A978D-EDD0-DB4B-AF38-97F4E8575985}" scale="150" hiddenColumns="1">
+      <selection activeCell="R6" sqref="A1:R6"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <hyperlinks>
-    <hyperlink ref="P4" r:id="rId1"/>
+    <hyperlink ref="P4" r:id="rId1" display="\\root{16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2210,25 +2494,496 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:AI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" customWidth="1"/>
+    <col min="19" max="20" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="2"/>
+    </row>
+    <row r="2" spans="1:35" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2">
+        <v>2</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AI2" s="2"/>
+    </row>
+    <row r="3" spans="1:35" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2">
+        <v>1</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AI3" s="2"/>
+    </row>
+    <row r="4" spans="1:35" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AI4" s="2"/>
+    </row>
+    <row r="5" spans="1:35" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5" t="s">
+        <v>127</v>
+      </c>
+      <c r="R5" s="2">
+        <v>2</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2">
+        <v>1</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
+      </c>
+      <c r="P7" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{A88A978D-EDD0-DB4B-AF38-97F4E8575985}" scale="150" hiddenColumns="1" topLeftCell="D1">
+      <selection activeCell="T3" sqref="T3"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM6"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -2275,15 +3030,15 @@
         <v>32</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -2292,63 +3047,64 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="M2" s="2"/>
       <c r="N2" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="O2" s="2">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
-        <v>67</v>
+      <c r="P2" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="Q2" s="2"/>
-      <c r="R2" s="2">
-        <v>0</v>
+      <c r="R2" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
       <c r="X2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AJ2" s="2"/>
-    </row>
-    <row r="3" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="Y2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AM2" s="2"/>
+    </row>
+    <row r="3" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -2357,63 +3113,64 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="M3" s="2"/>
       <c r="N3" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="O3">
         <v>2</v>
       </c>
-      <c r="P3" t="s">
-        <v>68</v>
+      <c r="P3" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="Q3" s="2"/>
-      <c r="R3" s="2">
-        <v>1</v>
+      <c r="R3" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
       <c r="X3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AJ3" s="2"/>
-    </row>
-    <row r="4" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="Y3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AM3" s="2"/>
+    </row>
+    <row r="4" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -2422,63 +3179,64 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="O4">
         <v>3</v>
       </c>
-      <c r="P4" t="s">
-        <v>69</v>
+      <c r="P4" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="Q4" s="2"/>
-      <c r="R4" s="2">
-        <v>1</v>
+      <c r="R4" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
       <c r="X4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AJ4" s="2"/>
-    </row>
-    <row r="5" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="Y4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AM4" s="2"/>
+    </row>
+    <row r="5" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -2487,54 +3245,56 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="M5" s="2"/>
       <c r="N5" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="O5">
         <v>4</v>
       </c>
-      <c r="P5" t="s">
-        <v>70</v>
-      </c>
-      <c r="R5" s="2">
-        <v>0</v>
+      <c r="P5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
-    </row>
-    <row r="6" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+    </row>
+    <row r="6" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
@@ -2543,55 +3303,486 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="M6" s="2"/>
       <c r="N6" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="O6">
         <v>5</v>
       </c>
-      <c r="P6" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2">
-        <v>1</v>
+      <c r="P6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
-    </row>
-    <row r="7" spans="1:36" ht="17" x14ac:dyDescent="0.2">
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:39" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>89</v>
+      </c>
+      <c r="T2" t="s">
+        <v>90</v>
+      </c>
+      <c r="U2" t="s">
+        <v>91</v>
+      </c>
+      <c r="V2" t="s">
+        <v>92</v>
+      </c>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AM2" s="2"/>
+    </row>
+    <row r="3" spans="1:39" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>93</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3" t="s">
+        <v>94</v>
+      </c>
+      <c r="T3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U3" t="s">
+        <v>96</v>
+      </c>
+      <c r="V3" t="s">
+        <v>97</v>
+      </c>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AM3" s="2"/>
+    </row>
+    <row r="4" spans="1:39" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" t="s">
+        <v>163</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>98</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4" t="s">
+        <v>99</v>
+      </c>
+      <c r="T4" t="s">
+        <v>100</v>
+      </c>
+      <c r="U4" t="s">
+        <v>101</v>
+      </c>
+      <c r="V4" t="s">
+        <v>102</v>
+      </c>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AM4" s="2"/>
+    </row>
+    <row r="5" spans="1:39" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" t="s">
+        <v>163</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5" t="s">
+        <v>103</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5" t="s">
+        <v>99</v>
+      </c>
+      <c r="T5" t="s">
+        <v>100</v>
+      </c>
+      <c r="U5" t="s">
+        <v>101</v>
+      </c>
+      <c r="V5" t="s">
+        <v>102</v>
+      </c>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+    </row>
+    <row r="6" spans="1:39" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" t="s">
+        <v>163</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6" t="s">
+        <v>104</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="S6" t="s">
+        <v>105</v>
+      </c>
+      <c r="T6" t="s">
+        <v>106</v>
+      </c>
+      <c r="U6" t="s">
+        <v>107</v>
+      </c>
+      <c r="V6" t="s">
+        <v>108</v>
+      </c>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+    </row>
+    <row r="7" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
@@ -2609,38 +3800,170 @@
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>66</v>
+        <v>87</v>
+      </c>
+      <c r="N7" t="s">
+        <v>163</v>
       </c>
       <c r="O7">
         <v>6</v>
       </c>
       <c r="P7" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2">
-        <v>1</v>
+        <v>109</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T7" t="s">
+        <v>111</v>
+      </c>
+      <c r="U7" t="s">
+        <v>112</v>
+      </c>
+      <c r="V7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N8" t="s">
+        <v>163</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
+      <c r="P8" t="s">
+        <v>114</v>
+      </c>
+      <c r="R8">
+        <v>3</v>
+      </c>
+      <c r="S8" t="s">
+        <v>115</v>
+      </c>
+      <c r="T8" t="s">
+        <v>116</v>
+      </c>
+      <c r="U8" t="s">
+        <v>117</v>
+      </c>
+      <c r="V8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N9" t="s">
+        <v>163</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
+      <c r="P9" t="s">
+        <v>119</v>
+      </c>
+      <c r="R9">
+        <v>3</v>
+      </c>
+      <c r="S9" t="s">
+        <v>118</v>
+      </c>
+      <c r="T9" t="s">
+        <v>116</v>
+      </c>
+      <c r="U9" t="s">
+        <v>117</v>
+      </c>
+      <c r="V9" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>